<commit_message>
Added New TestCase - TC_0002
</commit_message>
<xml_diff>
--- a/data/TC001 - Copy.xlsx
+++ b/data/TC001 - Copy.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TestLeaf\Desktop\Sample\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\workspace_1\Selenium-Practice\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA32271-12B6-41A9-A10D-3581CE1C8408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="15315" windowHeight="7590"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
+    <sheet name="Login" sheetId="8" r:id="rId1"/>
+    <sheet name="Create" sheetId="9" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Uname</t>
   </si>
@@ -34,12 +36,39 @@
   </si>
   <si>
     <t>DemoCSR</t>
+  </si>
+  <si>
+    <t>companyName</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>TestLeaf</t>
+  </si>
+  <si>
+    <t>TestFnameOne</t>
+  </si>
+  <si>
+    <t>TestLnameOne</t>
+  </si>
+  <si>
+    <t>LeafTab</t>
+  </si>
+  <si>
+    <t>TestFnameTwo</t>
+  </si>
+  <si>
+    <t>TestLnameTwo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -195,6 +224,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -230,6 +276,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -405,11 +468,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,4 +508,76 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95508D9B-0AEA-44E5-AF32-1D106D25ED1F}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added findLeads script - partially
</commit_message>
<xml_diff>
--- a/data/TC001 - Copy.xlsx
+++ b/data/TC001 - Copy.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\workspace_1\Selenium-Practice\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\workspace_1\Selenium-Practice\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA32271-12B6-41A9-A10D-3581CE1C8408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E92540-DB55-4975-8F38-CA4AB547879E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="8" r:id="rId1"/>
     <sheet name="Create" sheetId="9" r:id="rId2"/>
+    <sheet name="Find" sheetId="10" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
   <si>
     <t>Uname</t>
   </si>
@@ -514,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95508D9B-0AEA-44E5-AF32-1D106D25ED1F}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,4 +581,76 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E752D3BD-CC1F-44F9-AFD7-55AD11F87864}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Reporter logics and Updated code for Few testcases
</commit_message>
<xml_diff>
--- a/data/TC001 - Copy.xlsx
+++ b/data/TC001 - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\workspace_1\Selenium-Practice\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E92540-DB55-4975-8F38-CA4AB547879E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8164FD0F-F5EC-4AEE-A855-FA224A3F4AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t>Uname</t>
   </si>
@@ -39,31 +39,34 @@
     <t>DemoCSR</t>
   </si>
   <si>
-    <t>companyName</t>
-  </si>
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>TestLeaf</t>
-  </si>
-  <si>
-    <t>TestFnameOne</t>
-  </si>
-  <si>
-    <t>TestLnameOne</t>
-  </si>
-  <si>
-    <t>LeafTab</t>
-  </si>
-  <si>
-    <t>TestFnameTwo</t>
-  </si>
-  <si>
-    <t>TestLnameTwo</t>
+    <t>S.No</t>
+  </si>
+  <si>
+    <t>TC_0001</t>
+  </si>
+  <si>
+    <t>TC_0002</t>
+  </si>
+  <si>
+    <t>Test Description</t>
+  </si>
+  <si>
+    <t>Verify User is able to login</t>
+  </si>
+  <si>
+    <t>Verify User is able to login and logout</t>
+  </si>
+  <si>
+    <t>Verify User is able to create lead using DemoSalesManager login</t>
+  </si>
+  <si>
+    <t>Verify User is able to create lead using DemoCSR login</t>
+  </si>
+  <si>
+    <t>Verify User is able to create and find lead using DemoSalesManager login</t>
+  </si>
+  <si>
+    <t>Verify User is able to create and find lead using DemoCSR login</t>
   </si>
 </sst>
 </file>
@@ -470,38 +473,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -513,69 +537,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95508D9B-0AEA-44E5-AF32-1D106D25ED1F}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:E3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -585,69 +600,58 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E752D3BD-CC1F-44F9-AFD7-55AD11F87864}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>